<commit_message>
Make skipping tests more challenging (blank row btwn col names and data, plus another embedded blank row)
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/skipping.xlsx
+++ b/tests/testthat/sheets/skipping.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="8">
   <si>
     <t>blah blah</t>
   </si>
@@ -41,6 +41,18 @@
   </si>
   <si>
     <t>var2</t>
+  </si>
+  <si>
+    <t>v2,1</t>
+  </si>
+  <si>
+    <t>v2,2</t>
+  </si>
+  <si>
+    <t>v4,1</t>
+  </si>
+  <si>
+    <t>v4,2</t>
   </si>
 </sst>
 </file>
@@ -355,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B5"/>
+  <dimension ref="A3:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -371,20 +383,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-    </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>21</v>
-      </c>
-      <c r="B5">
-        <v>22</v>
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -394,10 +406,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -415,20 +427,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-    </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>21</v>
-      </c>
-      <c r="B5">
-        <v>22</v>
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -438,10 +450,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -464,20 +476,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-    </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>21</v>
-      </c>
-      <c r="B5">
-        <v>22</v>
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>